<commit_message>
Funciona a traves de un csv transformado a xlsx dinamicamente.
</commit_message>
<xml_diff>
--- a/project/output/informe_de_calidad.xlsx
+++ b/project/output/informe_de_calidad.xlsx
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7">
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8">
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +587,36 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fecha_invalida</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2906</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>fecha_invalidasatisf_fuera_rango</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>satisf_fuera_rango</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Versión final del proyecto con Quartz
</commit_message>
<xml_diff>
--- a/project/output/informe_de_calidad.xlsx
+++ b/project/output/informe_de_calidad.xlsx
@@ -449,37 +449,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>fecha</t>
+          <t>tienda</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>id_respuesta</t>
+          <t>satisfaccion</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>canal</t>
+          <t>comentario</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>producto</t>
+          <t>canal</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -489,31 +489,31 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>satisfaccion</t>
+          <t>id_respuesta</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>comentario</t>
+          <t>fecha</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>tienda</t>
+          <t>producto</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">

</xml_diff>